<commit_message>
Agregué una mochila nueva y también una nueva combinación
El digital Ruso.
</commit_message>
<xml_diff>
--- a/migracionWordPressPrestashop/Construccion de las Combinaciones.xlsx
+++ b/migracionWordPressPrestashop/Construccion de las Combinaciones.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="291">
   <si>
     <t>Modelo</t>
   </si>
@@ -167,9 +167,6 @@
     <t>Blanco</t>
   </si>
   <si>
-    <t>Selva Negra</t>
-  </si>
-  <si>
     <t>Color Simple</t>
   </si>
   <si>
@@ -885,6 +882,15 @@
   </si>
   <si>
     <t>Columna1</t>
+  </si>
+  <si>
+    <t>Digital Ruso</t>
+  </si>
+  <si>
+    <t>Camuflado</t>
+  </si>
+  <si>
+    <t>Multicam Negro</t>
   </si>
 </sst>
 </file>
@@ -1310,22 +1316,22 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -1344,72 +1350,72 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -1429,42 +1435,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -1477,7 +1483,7 @@
   <dimension ref="A1:J182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B23"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1490,57 +1496,57 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
         <v>74</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
         <v>75</v>
       </c>
-      <c r="C1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>76</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>242</v>
+      </c>
+      <c r="H1" t="s">
         <v>77</v>
       </c>
-      <c r="G1" t="s">
-        <v>243</v>
-      </c>
-      <c r="H1" t="s">
-        <v>78</v>
-      </c>
       <c r="I1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G2" t="s">
+        <v>245</v>
+      </c>
+      <c r="H2" t="s">
         <v>246</v>
       </c>
-      <c r="H2" t="s">
-        <v>247</v>
-      </c>
       <c r="I2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J2" t="str">
         <f>+Tabla1[[#This Row],[EQUIVALENCIA]]</f>
@@ -1555,25 +1561,25 @@
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J3" t="str">
         <f>+Tabla1[[#This Row],[EQUIVALENCIA]]</f>
@@ -1588,19 +1594,19 @@
         <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J4" t="str">
         <f>+Tabla1[[#This Row],[EQUIVALENCIA]]</f>
@@ -1615,13 +1621,13 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5">
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J5" t="str">
         <f>+Tabla1[[#This Row],[EQUIVALENCIA]]</f>
@@ -1636,13 +1642,13 @@
         <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6">
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J6" t="str">
         <f>+Tabla1[[#This Row],[EQUIVALENCIA]]</f>
@@ -1657,13 +1663,13 @@
         <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D7">
         <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J7" t="str">
         <f>+Tabla1[[#This Row],[EQUIVALENCIA]]</f>
@@ -1678,13 +1684,13 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D8">
         <v>6</v>
       </c>
       <c r="H8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J8" t="str">
         <f>+Tabla1[[#This Row],[EQUIVALENCIA]]</f>
@@ -1699,13 +1705,13 @@
         <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9">
         <v>7</v>
       </c>
       <c r="H9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J9" t="str">
         <f>+Tabla1[[#This Row],[EQUIVALENCIA]]</f>
@@ -1720,7 +1726,7 @@
         <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10">
         <v>8</v>
@@ -1738,7 +1744,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D11">
         <v>9</v>
@@ -1756,7 +1762,7 @@
         <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -1774,7 +1780,7 @@
         <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D13">
         <v>11</v>
@@ -1893,6 +1899,9 @@
       <c r="A21" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="B21" t="s">
+        <v>289</v>
+      </c>
       <c r="D21">
         <v>19</v>
       </c>
@@ -1921,7 +1930,7 @@
         <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>290</v>
       </c>
       <c r="D23">
         <v>21</v>
@@ -1933,7 +1942,10 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="B24" t="s">
+        <v>53</v>
       </c>
       <c r="D24">
         <v>22</v>
@@ -1945,7 +1957,10 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="B25" t="s">
+        <v>288</v>
       </c>
       <c r="D25">
         <v>23</v>
@@ -1957,7 +1972,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D26">
         <v>24</v>
@@ -1969,7 +1984,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D27">
         <v>25</v>
@@ -1981,7 +1996,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D28">
         <v>26</v>
@@ -1993,7 +2008,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D29">
         <v>27</v>
@@ -2005,7 +2020,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D30">
         <v>28</v>
@@ -2017,7 +2032,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D31">
         <v>29</v>
@@ -2029,7 +2044,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D32">
         <v>30</v>
@@ -2041,7 +2056,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D33">
         <v>31</v>
@@ -2053,7 +2068,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D34">
         <v>32</v>
@@ -2065,7 +2080,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D35">
         <v>33</v>
@@ -2077,7 +2092,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D36">
         <v>34</v>
@@ -2089,7 +2104,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D37">
         <v>35</v>
@@ -2101,7 +2116,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D38">
         <v>36</v>
@@ -2113,7 +2128,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D39">
         <v>37</v>
@@ -2125,7 +2140,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D40">
         <v>38</v>
@@ -2137,7 +2152,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D41">
         <v>39</v>
@@ -2149,7 +2164,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D42">
         <v>40</v>
@@ -2161,7 +2176,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D43">
         <v>41</v>
@@ -2173,7 +2188,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D44">
         <v>42</v>
@@ -2185,7 +2200,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D45">
         <v>43</v>
@@ -2197,7 +2212,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D46">
         <v>44</v>
@@ -2209,7 +2224,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D47">
         <v>45</v>
@@ -2221,7 +2236,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D48">
         <v>46</v>
@@ -2233,7 +2248,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D49">
         <v>47</v>
@@ -2245,7 +2260,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D50">
         <v>48</v>
@@ -2257,7 +2272,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D51">
         <v>49</v>
@@ -2269,7 +2284,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D52">
         <v>50</v>
@@ -2281,7 +2296,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D53">
         <v>51</v>
@@ -2293,7 +2308,7 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D54">
         <v>52</v>
@@ -2305,7 +2320,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D55">
         <v>53</v>
@@ -2317,7 +2332,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D56">
         <v>54</v>
@@ -2329,7 +2344,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D57">
         <v>55</v>
@@ -2341,7 +2356,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D58">
         <v>56</v>
@@ -2353,7 +2368,7 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D59">
         <v>57</v>
@@ -2365,7 +2380,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D60">
         <v>58</v>
@@ -2377,7 +2392,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D61">
         <v>59</v>
@@ -2389,7 +2404,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D62">
         <v>60</v>
@@ -2401,7 +2416,7 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D63">
         <v>61</v>
@@ -2413,7 +2428,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D64">
         <v>62</v>
@@ -2425,7 +2440,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D65">
         <v>63</v>
@@ -2437,7 +2452,7 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D66">
         <v>64</v>
@@ -2449,7 +2464,7 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D67">
         <v>65</v>
@@ -2461,7 +2476,7 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D68">
         <v>66</v>
@@ -2473,7 +2488,7 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D69">
         <v>67</v>
@@ -2485,7 +2500,7 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D70">
         <v>68</v>
@@ -2497,7 +2512,7 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D71">
         <v>69</v>
@@ -2509,7 +2524,7 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D72">
         <v>70</v>
@@ -2521,7 +2536,7 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D73">
         <v>71</v>
@@ -2533,7 +2548,7 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D74">
         <v>72</v>
@@ -2545,7 +2560,7 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D75">
         <v>73</v>
@@ -2557,7 +2572,7 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D76">
         <v>74</v>
@@ -2569,7 +2584,7 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D77">
         <v>75</v>
@@ -2581,7 +2596,7 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D78">
         <v>76</v>
@@ -2593,7 +2608,7 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D79">
         <v>77</v>
@@ -2605,7 +2620,7 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D80">
         <v>78</v>
@@ -2617,7 +2632,7 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D81">
         <v>79</v>
@@ -2629,7 +2644,7 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D82">
         <v>80</v>
@@ -2641,7 +2656,7 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D83">
         <v>81</v>
@@ -2653,7 +2668,7 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D84">
         <v>82</v>
@@ -2665,7 +2680,7 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D85">
         <v>83</v>
@@ -2677,7 +2692,7 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D86">
         <v>84</v>
@@ -2689,7 +2704,7 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D87">
         <v>85</v>
@@ -2701,7 +2716,7 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D88">
         <v>86</v>
@@ -2713,7 +2728,7 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D89">
         <v>87</v>
@@ -2725,7 +2740,7 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D90">
         <v>88</v>
@@ -2737,7 +2752,7 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D91">
         <v>89</v>
@@ -2749,7 +2764,7 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D92">
         <v>90</v>
@@ -2761,7 +2776,7 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D93">
         <v>91</v>
@@ -2773,7 +2788,7 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D94">
         <v>92</v>
@@ -2785,7 +2800,7 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D95">
         <v>93</v>
@@ -2797,7 +2812,7 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D96">
         <v>94</v>
@@ -2809,7 +2824,7 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D97">
         <v>95</v>
@@ -2821,7 +2836,7 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D98">
         <v>96</v>
@@ -2833,7 +2848,7 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D99">
         <v>97</v>
@@ -2845,7 +2860,7 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D100">
         <v>98</v>
@@ -2857,7 +2872,7 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D101">
         <v>99</v>
@@ -2869,7 +2884,7 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D102">
         <v>100</v>
@@ -2881,7 +2896,7 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D103">
         <v>101</v>
@@ -2893,7 +2908,7 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D104">
         <v>102</v>
@@ -2905,7 +2920,7 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D105">
         <v>103</v>
@@ -2917,7 +2932,7 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D106">
         <v>104</v>
@@ -2929,7 +2944,7 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D107">
         <v>105</v>
@@ -2941,7 +2956,7 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D108">
         <v>106</v>
@@ -2953,7 +2968,7 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D109">
         <v>107</v>
@@ -2965,7 +2980,7 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D110">
         <v>108</v>
@@ -2977,7 +2992,7 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D111">
         <v>109</v>
@@ -2989,7 +3004,7 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D112">
         <v>110</v>
@@ -3001,7 +3016,7 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D113">
         <v>111</v>
@@ -3013,7 +3028,7 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D114">
         <v>112</v>
@@ -3025,7 +3040,7 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D115">
         <v>113</v>
@@ -3037,7 +3052,7 @@
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D116">
         <v>114</v>
@@ -3049,7 +3064,7 @@
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D117">
         <v>115</v>
@@ -3061,7 +3076,7 @@
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D118">
         <v>116</v>
@@ -3073,7 +3088,7 @@
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D119">
         <v>117</v>
@@ -3085,7 +3100,7 @@
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D120">
         <v>118</v>
@@ -3097,7 +3112,7 @@
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D121">
         <v>119</v>
@@ -3109,7 +3124,7 @@
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D122">
         <v>120</v>
@@ -3121,7 +3136,7 @@
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D123">
         <v>121</v>
@@ -3133,7 +3148,7 @@
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D124">
         <v>122</v>
@@ -3145,7 +3160,7 @@
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D125">
         <v>123</v>
@@ -3157,7 +3172,7 @@
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D126">
         <v>124</v>
@@ -3169,7 +3184,7 @@
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D127">
         <v>125</v>
@@ -3181,7 +3196,7 @@
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D128">
         <v>126</v>
@@ -3193,7 +3208,7 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D129">
         <v>127</v>
@@ -3205,7 +3220,7 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D130">
         <v>128</v>
@@ -3217,7 +3232,7 @@
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D131">
         <v>129</v>
@@ -3229,7 +3244,7 @@
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D132">
         <v>130</v>
@@ -3241,7 +3256,7 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D133">
         <v>131</v>
@@ -3253,7 +3268,7 @@
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D134">
         <v>132</v>
@@ -3265,7 +3280,7 @@
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D135">
         <v>133</v>
@@ -3277,7 +3292,7 @@
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D136">
         <v>134</v>
@@ -3289,7 +3304,7 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D137">
         <v>135</v>
@@ -3301,7 +3316,7 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D138">
         <v>136</v>
@@ -3313,7 +3328,7 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D139">
         <v>137</v>
@@ -3325,7 +3340,7 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D140">
         <v>138</v>
@@ -3337,7 +3352,7 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D141">
         <v>139</v>
@@ -3349,7 +3364,7 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D142">
         <v>140</v>
@@ -3361,7 +3376,7 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D143">
         <v>141</v>
@@ -3373,7 +3388,7 @@
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D144">
         <v>142</v>
@@ -3385,7 +3400,7 @@
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D145">
         <v>143</v>
@@ -3397,7 +3412,7 @@
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D146">
         <v>144</v>
@@ -3409,7 +3424,7 @@
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D147">
         <v>145</v>
@@ -3421,7 +3436,7 @@
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D148">
         <v>146</v>
@@ -3433,7 +3448,7 @@
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D149">
         <v>147</v>
@@ -3445,7 +3460,7 @@
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D150">
         <v>148</v>
@@ -3457,7 +3472,7 @@
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D151">
         <v>149</v>
@@ -3469,7 +3484,7 @@
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D152">
         <v>150</v>
@@ -3481,7 +3496,7 @@
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D153">
         <v>151</v>
@@ -3493,7 +3508,7 @@
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D154">
         <v>152</v>
@@ -3505,7 +3520,7 @@
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D155">
         <v>153</v>
@@ -3517,7 +3532,7 @@
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D156">
         <v>154</v>
@@ -3529,7 +3544,7 @@
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D157">
         <v>155</v>
@@ -3541,7 +3556,7 @@
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D158">
         <v>156</v>
@@ -3553,7 +3568,7 @@
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D159">
         <v>157</v>
@@ -3565,7 +3580,7 @@
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D160">
         <v>158</v>
@@ -3577,7 +3592,7 @@
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D161">
         <v>159</v>
@@ -3589,7 +3604,7 @@
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D162">
         <v>160</v>
@@ -3601,7 +3616,7 @@
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D163">
         <v>161</v>
@@ -3613,7 +3628,7 @@
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D164">
         <v>162</v>
@@ -3625,7 +3640,7 @@
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D165">
         <v>163</v>
@@ -3637,7 +3652,7 @@
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D166">
         <v>164</v>
@@ -3649,7 +3664,7 @@
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D167">
         <v>165</v>
@@ -3661,7 +3676,7 @@
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D168">
         <v>166</v>
@@ -3673,7 +3688,7 @@
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D169">
         <v>167</v>
@@ -3685,7 +3700,7 @@
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D170">
         <v>168</v>
@@ -3697,7 +3712,7 @@
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D171">
         <v>169</v>
@@ -3709,7 +3724,7 @@
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D172">
         <v>170</v>
@@ -3721,7 +3736,7 @@
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D173">
         <v>171</v>
@@ -3733,7 +3748,7 @@
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D174">
         <v>172</v>
@@ -3745,7 +3760,7 @@
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D175">
         <v>173</v>
@@ -3757,7 +3772,7 @@
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D176">
         <v>174</v>
@@ -3769,7 +3784,7 @@
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D177">
         <v>175</v>
@@ -3781,7 +3796,7 @@
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D178">
         <v>176</v>
@@ -3793,7 +3808,7 @@
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D179">
         <v>177</v>
@@ -3805,7 +3820,7 @@
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D180">
         <v>178</v>
@@ -3817,7 +3832,7 @@
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D181">
         <v>179</v>
@@ -3829,7 +3844,7 @@
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D182">
         <v>180</v>
@@ -3859,7 +3874,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -3894,17 +3909,17 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
@@ -3914,37 +3929,37 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>